<commit_message>
entity reference => uriorcurie
</commit_message>
<xml_diff>
--- a/project/excel/sssom_schema.xlsx
+++ b/project/excel/sssom_schema.xlsx
@@ -1,17 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="4" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="7" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="EntityReference" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Mapping" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="MappingRegistry" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="MappingSet" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="MappingSetReference" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Mapping" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MappingRegistry" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MappingSet" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MappingSetReference" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Mapping1" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MappingRegistry1" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MappingSet1" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MappingSetReference1" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -417,19 +420,475 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:AN1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>subject_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>subject_label</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>subject_category</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>predicate_id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>predicate_label</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>predicate_modifier</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>object_id</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>object_label</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>object_category</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>mapping_justification</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>author_id</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>author_label</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>reviewer_id</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>reviewer_label</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>creator_id</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>creator_label</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>license</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>subject_type</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>subject_source</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>subject_source_version</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>object_type</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>object_source</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>object_source_version</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>mapping_provider</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>mapping_source</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>mapping_cardinality</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>mapping_tool</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>mapping_tool_version</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>mapping_date</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>confidence</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>subject_match_field</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>object_match_field</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>match_string</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>subject_preprocessing</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>object_preprocessing</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>semantic_similarity_score</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>semantic_similarity_measure</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>see_also</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>mapping_registry_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>mapping_registry_title</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>mapping_registry_description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>imports</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>mapping_set_references</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>documentation</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>homepage</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Y1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>mappings</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>mapping_set_id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>mapping_set_version</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>mapping_set_source</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>mapping_set_title</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>mapping_set_description</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>creator_id</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>creator_label</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>mapping set_license</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>subject_type</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>subject_source</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>subject_source_version</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>object_type</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>object_source</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>object_source_version</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>mapping_provider</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>mapping_tool</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>mapping_date</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>subject_match_field</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>object_match_field</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>subject_preprocessing</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>object_preprocessing</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>see_also</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>mapping_set_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>mirror_from</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>registry_confidence</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>mapping_set_group</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>last_updated</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>local_name</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -650,7 +1109,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -706,7 +1165,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -852,7 +1311,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
SSSOM 0.11.1 release (#270)
Recreating the SSSOM schema files

---------

Co-authored-by: Harshad Hegde <hegdehb@gmail.com>
</commit_message>
<xml_diff>
--- a/project/excel/sssom_schema.xlsx
+++ b/project/excel/sssom_schema.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Mapping" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MappingRegistry" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MappingSet" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MappingSetReference" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Mapping" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="MappingRegistry" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="MappingSet" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="MappingSetReference" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AM1"/>
+  <dimension ref="A1:AP1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -547,75 +547,90 @@
       </c>
       <c r="Y1" t="inlineStr">
         <is>
+          <t>mapping_source</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
           <t>mapping_cardinality</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>mapping_tool</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>mapping_tool_version</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>mapping_date</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>confidence</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>curation_rule</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>curation_rule_text</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
         <is>
           <t>subject_match_field</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>object_match_field</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>match_string</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>subject_preprocessing</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>object_preprocessing</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>semantic_similarity_score</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>semantic_similarity_measure</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>see_also</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>other</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>comment</t>
         </is>
@@ -632,7 +647,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -648,20 +663,30 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>mapping_registry_title</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>mapping_registry_description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>imports</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>mapping_set_references</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>documentation</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>homepage</t>
         </is>
@@ -678,7 +703,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X1"/>
+  <dimension ref="A1:Y1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -709,100 +734,105 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>mapping_set_title</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>mapping_set_description</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>creator_id</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>creator_label</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>mapping set_license</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>subject_type</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>subject_source</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>subject_source_version</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>object_type</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>object_source</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>object_source_version</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>mapping_provider</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>mapping_tool</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>mapping_date</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>subject_match_field</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>object_match_field</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>subject_preprocessing</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>object_preprocessing</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>see_also</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>other</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>comment</t>
         </is>

</xml_diff>

<commit_message>
ran make all again
</commit_message>
<xml_diff>
--- a/project/excel/sssom_schema.xlsx
+++ b/project/excel/sssom_schema.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Mapping" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="MappingRegistry" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="MappingSet" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="MappingSetReference" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Mapping" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MappingRegistry" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MappingSet" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MappingSetReference" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Issues around canonical ordering (#285)
Partially adresses #283 

- [X] `docs/` have been added/updated if necessary
- [X]
[CHANGELOG.md](https://github.com/mapping-commons/sssom/blob/master/CHANGELOG.md)
has been updated.

- Applies canonical sort ordering to all examples files
- Downgrades the necessity of applying the canonical column order from
MUST to SHOULD
- Documents clearly that built-in prefixes MUST NOT be redefined

---------

Co-authored-by: Harshad Hegde <hegdehb@gmail.com>
</commit_message>
<xml_diff>
--- a/project/excel/sssom_schema.xlsx
+++ b/project/excel/sssom_schema.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Mapping" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="MappingRegistry" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="MappingSet" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="MappingSetReference" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Mapping" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MappingRegistry" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MappingSet" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MappingSetReference" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Run `make all` (#303)
This PR does not change the underlying schema, it just runs `make all`

This also motivates some kind of CI check that when the schema is
updated, then this gets run.

I want to do this to reduce spurious diff in #302
</commit_message>
<xml_diff>
--- a/project/excel/sssom_schema.xlsx
+++ b/project/excel/sssom_schema.xlsx
@@ -4,13 +4,13 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Mapping" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MappingRegistry" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MappingSet" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MappingSetReference" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="mapping set" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="mapping" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="mapping registry" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="mapping set reference" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -416,6 +416,165 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:Z1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>mappings</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>mapping_set_id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>mapping_set_version</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>mapping_set_source</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>mapping_set_title</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>mapping_set_description</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>creator_id</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>creator_label</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>license</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>subject_type</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>subject_source</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>subject_source_version</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>object_type</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>object_source</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>object_source_version</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>mapping_provider</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>mapping_tool</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>mapping_tool_version</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>mapping_date</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>subject_match_field</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>object_match_field</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>subject_preprocessing</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>object_preprocessing</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>see_also</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation sqref="J2:J1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"owl class,owl object property,owl data property,owl annotation property,owl named individual,skos concept,rdfs resource,rdfs class,rdfs literal,rdfs datatype,rdf property"</formula1>
+    </dataValidation>
+    <dataValidation sqref="M2:M1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"owl class,owl object property,owl data property,owl annotation property,owl named individual,skos concept,rdfs resource,rdfs class,rdfs literal,rdfs datatype,rdf property"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:AP1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -637,11 +796,25 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="4">
+    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Not"</formula1>
+    </dataValidation>
+    <dataValidation sqref="R2:R1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"owl class,owl object property,owl data property,owl annotation property,owl named individual,skos concept,rdfs resource,rdfs class,rdfs literal,rdfs datatype,rdf property"</formula1>
+    </dataValidation>
+    <dataValidation sqref="U2:U1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"owl class,owl object property,owl data property,owl annotation property,owl named individual,skos concept,rdfs resource,rdfs class,rdfs literal,rdfs datatype,rdf property"</formula1>
+    </dataValidation>
+    <dataValidation sqref="Z2:Z1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"1:1,1:n,n:1,1:0,0:1,n:n"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -689,152 +862,6 @@
       <c r="G1" t="inlineStr">
         <is>
           <t>homepage</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:Y1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>mappings</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>mapping_set_id</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>mapping_set_version</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>mapping_set_source</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>mapping_set_title</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>mapping_set_description</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>creator_id</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>creator_label</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>mapping set_license</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>subject_type</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>subject_source</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>subject_source_version</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>object_type</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>object_source</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>object_source_version</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>mapping_provider</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>mapping_tool</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>mapping_date</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>subject_match_field</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>object_match_field</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>subject_preprocessing</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>object_preprocessing</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>see_also</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>other</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>comment</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Rebuilding documentation and generated files with Github Action
</commit_message>
<xml_diff>
--- a/project/excel/sssom_schema.xlsx
+++ b/project/excel/sssom_schema.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="mapping set" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="mapping" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="mapping registry" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="mapping set reference" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Mapping" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="MappingRegistry" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="MappingSet" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="MappingSetReference" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z1"/>
+  <dimension ref="A1:AR1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -427,144 +427,226 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>mappings</t>
+          <t>subject_id</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>mapping_set_id</t>
+          <t>subject_label</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>mapping_set_version</t>
+          <t>subject_category</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>mapping_set_source</t>
+          <t>predicate_id</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>mapping_set_title</t>
+          <t>predicate_label</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>mapping_set_description</t>
+          <t>predicate_modifier</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
+          <t>object_id</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>object_label</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>object_category</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>mapping_justification</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>author_id</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>author_label</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>reviewer_id</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>reviewer_label</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
           <t>creator_id</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>creator_label</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>license</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>subject_type</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>subject_source</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>subject_source_version</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>object_type</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>object_source</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>object_source_version</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>mapping_provider</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>mapping_source</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>mapping_cardinality</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
         <is>
           <t>mapping_tool</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>mapping_tool_version</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>mapping_date</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>publication_date</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>confidence</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>curation_rule</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>curation_rule_text</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
         <is>
           <t>subject_match_field</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>object_match_field</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>match_string</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
         <is>
           <t>subject_preprocessing</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>object_preprocessing</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>semantic_similarity_score</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>semantic_similarity_measure</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
         <is>
           <t>see_also</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>issue_tracker_item</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>other</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>comment</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation sqref="J2:J1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"owl class,owl object property,owl data property,owl annotation property,owl named individual,skos concept,rdfs resource,rdfs class,rdfs literal,rdfs datatype,rdf property"</formula1>
-    </dataValidation>
-    <dataValidation sqref="M2:M1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"owl class,owl object property,owl data property,owl annotation property,owl named individual,skos concept,rdfs resource,rdfs class,rdfs literal,rdfs datatype,rdf property"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -575,7 +657,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AP1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -586,230 +668,46 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>subject_id</t>
+          <t>mapping_registry_id</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>subject_label</t>
+          <t>mapping_registry_title</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>subject_category</t>
+          <t>mapping_registry_description</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>predicate_id</t>
+          <t>imports</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>predicate_label</t>
+          <t>mapping_set_references</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>predicate_modifier</t>
+          <t>documentation</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>object_id</t>
+          <t>homepage</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>object_label</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>object_category</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>mapping_justification</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>author_id</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>author_label</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>reviewer_id</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>reviewer_label</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>creator_id</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>creator_label</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>license</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>subject_type</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>subject_source</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>subject_source_version</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>object_type</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>object_source</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>object_source_version</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>mapping_provider</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>mapping_source</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>mapping_cardinality</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>mapping_tool</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>mapping_tool_version</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>mapping_date</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>confidence</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>curation_rule</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>curation_rule_text</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>subject_match_field</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>object_match_field</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>match_string</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>subject_preprocessing</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>object_preprocessing</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>semantic_similarity_score</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>semantic_similarity_measure</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
-        <is>
-          <t>see_also</t>
-        </is>
-      </c>
-      <c r="AO1" t="inlineStr">
-        <is>
-          <t>other</t>
-        </is>
-      </c>
-      <c r="AP1" t="inlineStr">
-        <is>
-          <t>comment</t>
+          <t>issue_tracker</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"Not"</formula1>
-    </dataValidation>
-    <dataValidation sqref="R2:R1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"owl class,owl object property,owl data property,owl annotation property,owl named individual,skos concept,rdfs resource,rdfs class,rdfs literal,rdfs datatype,rdf property"</formula1>
-    </dataValidation>
-    <dataValidation sqref="U2:U1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"owl class,owl object property,owl data property,owl annotation property,owl named individual,skos concept,rdfs resource,rdfs class,rdfs literal,rdfs datatype,rdf property"</formula1>
-    </dataValidation>
-    <dataValidation sqref="Z2:Z1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"1:1,1:n,n:1,1:0,0:1,n:n"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -820,7 +718,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:AB1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -831,37 +729,142 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>mapping_registry_id</t>
+          <t>mappings</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>mapping_registry_title</t>
+          <t>mapping_set_id</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>mapping_registry_description</t>
+          <t>mapping_set_version</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>imports</t>
+          <t>mapping_set_source</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>mapping_set_references</t>
+          <t>mapping_set_title</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>documentation</t>
+          <t>mapping_set_description</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>homepage</t>
+          <t>creator_id</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>creator_label</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>mapping set_license</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>subject_type</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>subject_source</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>subject_source_version</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>object_type</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>object_source</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>object_source_version</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>mapping_provider</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>mapping_tool</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>mapping_tool_version</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>mapping_date</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>publication_date</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>subject_match_field</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>object_match_field</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>subject_preprocessing</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>object_preprocessing</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>see_also</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>issue_tracker</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>comment</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Regenerated schema files for pydantic branch
</commit_message>
<xml_diff>
--- a/project/excel/sssom_schema.xlsx
+++ b/project/excel/sssom_schema.xlsx
@@ -4,13 +4,15 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Mapping" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="MappingRegistry" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="MappingSet" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="MappingSetReference" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="mapping set" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="mapping" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="literal mapping" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="mapping registry" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="mapping set reference" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Propagatable" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -416,6 +418,175 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:AB1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>mappings</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>mapping_set_id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>mapping_set_version</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>mapping_set_source</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>mapping_set_title</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>mapping_set_description</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>creator_id</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>creator_label</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>license</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>subject_type</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>subject_source</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>subject_source_version</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>object_type</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>object_source</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>object_source_version</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>mapping_provider</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>mapping_tool</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>mapping_tool_version</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>mapping_date</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>publication_date</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>subject_match_field</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>object_match_field</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>subject_preprocessing</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>object_preprocessing</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>see_also</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>issue_tracker</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation sqref="J2:J1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"owl class,owl object property,owl data property,owl annotation property,owl named individual,skos concept,rdfs resource,rdfs class,rdfs literal,rdfs datatype,rdf property"</formula1>
+    </dataValidation>
+    <dataValidation sqref="M2:M1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"owl class,owl object property,owl data property,owl annotation property,owl named individual,skos concept,rdfs resource,rdfs class,rdfs literal,rdfs datatype,rdf property"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:AR1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -647,11 +818,242 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="4">
+    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Not"</formula1>
+    </dataValidation>
+    <dataValidation sqref="R2:R1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"owl class,owl object property,owl data property,owl annotation property,owl named individual,skos concept,rdfs resource,rdfs class,rdfs literal,rdfs datatype,rdf property"</formula1>
+    </dataValidation>
+    <dataValidation sqref="U2:U1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"owl class,owl object property,owl data property,owl annotation property,owl named individual,skos concept,rdfs resource,rdfs class,rdfs literal,rdfs datatype,rdf property"</formula1>
+    </dataValidation>
+    <dataValidation sqref="Z2:Z1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"1:1,1:n,n:1,1:0,0:1,n:n"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AK1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>literal</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>literal_datatype</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>predicate_id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>predicate_label</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>predicate_modifier</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>object_id</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>object_label</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>object_category</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>mapping_justification</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>author_id</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>author_label</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>reviewer_id</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>reviewer_label</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>creator_id</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>creator_label</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>license</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>literal_source</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>literal_source_version</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>object_type</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>object_source</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>object_source_version</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>mapping_provider</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>mapping_source</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>mapping_cardinality</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>mapping_tool</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>mapping_tool_version</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>mapping_date</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>confidence</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>object_match_field</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>match_string</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>literal_preprocessing</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>object_preprocessing</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>similarity_score</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>similarity_measure</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>see_also</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Not"</formula1>
+    </dataValidation>
+    <dataValidation sqref="S2:S1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"owl class,owl object property,owl data property,owl annotation property,owl named individual,skos concept,rdfs resource,rdfs class,rdfs literal,rdfs datatype,rdf property"</formula1>
+    </dataValidation>
+    <dataValidation sqref="X2:X1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"1:1,1:n,n:1,1:0,0:1,n:n"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -712,168 +1114,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AB1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>mappings</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>mapping_set_id</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>mapping_set_version</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>mapping_set_source</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>mapping_set_title</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>mapping_set_description</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>creator_id</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>creator_label</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>mapping set_license</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>subject_type</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>subject_source</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>subject_source_version</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>object_type</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>object_source</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>object_source_version</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>mapping_provider</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>mapping_tool</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>mapping_tool_version</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>mapping_date</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>publication_date</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>subject_match_field</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>object_match_field</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>subject_preprocessing</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>object_preprocessing</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>see_also</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>issue_tracker</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>other</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>comment</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -922,4 +1163,30 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>propagated</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add support for extension slots (#375)
This commit updates the SSSOM model to allow for _defined extensions_ as
proposed in #328.

It also updates the description of the data model to describe the use of
both defined and undefined extension, and the specification of the
SSSOM/TSV format to explain how SSSOM/TSV parsers and writers should
deal with such extensions.

Overall, this is exactly what was proposed in [this
comment](https://github.com/mapping-commons/sssom/issues/328#issuecomment-1879735143)
in #328, except that here we need to split the specification in two
parts (one about extensions in general, independently of the
serialisation format, and one about the SSSOM/TSV serialisation of
extensions), while the initial proposition was in a single block.

Co-authored-by: Nico Matentzoglu <nicolas.matentzoglu@gmail.com>
</commit_message>
<xml_diff>
--- a/project/excel/sssom_schema.xlsx
+++ b/project/excel/sssom_schema.xlsx
@@ -4,13 +4,16 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Mapping" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="MappingRegistry" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="MappingSet" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="MappingSetReference" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="mapping set" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="mapping" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="literal mapping" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="mapping registry" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="mapping set reference" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="extension definition" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Propagatable" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -416,6 +419,180 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:AC1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>mappings</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>mapping_set_id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>mapping_set_version</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>mapping_set_source</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>mapping_set_title</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>mapping_set_description</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>creator_id</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>creator_label</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>license</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>subject_type</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>subject_source</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>subject_source_version</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>object_type</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>object_source</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>object_source_version</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>mapping_provider</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>mapping_tool</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>mapping_tool_version</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>mapping_date</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>publication_date</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>subject_match_field</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>object_match_field</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>subject_preprocessing</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>object_preprocessing</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>see_also</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>issue_tracker</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>extension_definitions</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation sqref="J2:J1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"owl class,owl object property,owl data property,owl annotation property,owl named individual,skos concept,rdfs resource,rdfs class,rdfs literal,rdfs datatype,rdf property"</formula1>
+    </dataValidation>
+    <dataValidation sqref="M2:M1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"owl class,owl object property,owl data property,owl annotation property,owl named individual,skos concept,rdfs resource,rdfs class,rdfs literal,rdfs datatype,rdf property"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:AR1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -647,11 +824,242 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="4">
+    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Not"</formula1>
+    </dataValidation>
+    <dataValidation sqref="R2:R1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"owl class,owl object property,owl data property,owl annotation property,owl named individual,skos concept,rdfs resource,rdfs class,rdfs literal,rdfs datatype,rdf property"</formula1>
+    </dataValidation>
+    <dataValidation sqref="U2:U1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"owl class,owl object property,owl data property,owl annotation property,owl named individual,skos concept,rdfs resource,rdfs class,rdfs literal,rdfs datatype,rdf property"</formula1>
+    </dataValidation>
+    <dataValidation sqref="Z2:Z1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"1:1,1:n,n:1,1:0,0:1,n:n"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AK1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>literal</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>literal_datatype</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>predicate_id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>predicate_label</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>predicate_modifier</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>object_id</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>object_label</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>object_category</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>mapping_justification</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>author_id</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>author_label</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>reviewer_id</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>reviewer_label</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>creator_id</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>creator_label</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>license</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>literal_source</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>literal_source_version</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>object_type</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>object_source</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>object_source_version</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>mapping_provider</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>mapping_source</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>mapping_cardinality</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>mapping_tool</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>mapping_tool_version</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>mapping_date</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>confidence</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>object_match_field</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>match_string</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>literal_preprocessing</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>object_preprocessing</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>similarity_score</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>similarity_measure</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>see_also</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Not"</formula1>
+    </dataValidation>
+    <dataValidation sqref="S2:S1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"owl class,owl object property,owl data property,owl annotation property,owl named individual,skos concept,rdfs resource,rdfs class,rdfs literal,rdfs datatype,rdf property"</formula1>
+    </dataValidation>
+    <dataValidation sqref="X2:X1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"1:1,1:n,n:1,1:0,0:1,n:n"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -712,168 +1120,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AB1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>mappings</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>mapping_set_id</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>mapping_set_version</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>mapping_set_source</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>mapping_set_title</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>mapping_set_description</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>creator_id</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>creator_label</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>mapping set_license</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>subject_type</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>subject_source</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>subject_source_version</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>object_type</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>object_source</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>object_source_version</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>mapping_provider</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>mapping_tool</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>mapping_tool_version</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>mapping_date</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>publication_date</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>subject_match_field</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>object_match_field</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>subject_preprocessing</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>object_preprocessing</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>see_also</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>issue_tracker</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>other</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>comment</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -922,4 +1169,66 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>slot_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>property</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>type_hint</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>propagated</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add `curie_map` to the model (#376)
This commit makes the `curie_map` a _bona fide_ slot of the `MappingSet`
class, that exists independently of the serialisation format.

---------

Co-authored-by: Nico Matentzoglu <nicolas.matentzoglu@gmail.com>
</commit_message>
<xml_diff>
--- a/project/excel/sssom_schema.xlsx
+++ b/project/excel/sssom_schema.xlsx
@@ -9,11 +9,12 @@
   <sheets>
     <sheet name="mapping set" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="mapping" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="literal mapping" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="mapping registry" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="mapping set reference" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="mapping registry" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="mapping set reference" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="prefix" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="extension definition" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="Propagatable" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="NoTermFound" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -419,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC1"/>
+  <dimension ref="A1:AD1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -430,145 +431,150 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>curie_map</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>mappings</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>mapping_set_id</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>mapping_set_version</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>mapping_set_source</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>mapping_set_title</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>mapping_set_description</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>creator_id</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>creator_label</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>license</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>subject_type</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>subject_source</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>subject_source_version</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>object_type</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>object_source</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>object_source_version</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>mapping_provider</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>mapping_tool</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>mapping_tool_version</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>mapping_date</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>publication_date</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>subject_match_field</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>object_match_field</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>subject_preprocessing</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>object_preprocessing</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>see_also</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>issue_tracker</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>other</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>comment</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>extension_definitions</t>
         </is>
@@ -576,10 +582,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation sqref="J2:J1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="K2:K1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"owl class,owl object property,owl data property,owl annotation property,owl named individual,skos concept,rdfs resource,rdfs class,rdfs literal,rdfs datatype,rdf property"</formula1>
     </dataValidation>
-    <dataValidation sqref="M2:M1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="N2:N1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"owl class,owl object property,owl data property,owl annotation property,owl named individual,skos concept,rdfs resource,rdfs class,rdfs literal,rdfs datatype,rdf property"</formula1>
     </dataValidation>
   </dataValidations>
@@ -794,12 +800,12 @@
       </c>
       <c r="AM1" t="inlineStr">
         <is>
-          <t>semantic_similarity_score</t>
+          <t>similarity_score</t>
         </is>
       </c>
       <c r="AN1" t="inlineStr">
         <is>
-          <t>semantic_similarity_measure</t>
+          <t>similarity_measure</t>
         </is>
       </c>
       <c r="AO1" t="inlineStr">
@@ -848,223 +854,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AK1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>literal</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>literal_datatype</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>predicate_id</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>predicate_label</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>predicate_modifier</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>object_id</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>object_label</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>object_category</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>mapping_justification</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>author_id</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>author_label</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>reviewer_id</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>reviewer_label</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>creator_id</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>creator_label</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>license</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>literal_source</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>literal_source_version</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>object_type</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>object_source</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>object_source_version</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>mapping_provider</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>mapping_source</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>mapping_cardinality</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>mapping_tool</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>mapping_tool_version</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>mapping_date</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>confidence</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>object_match_field</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>match_string</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>literal_preprocessing</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>object_preprocessing</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>similarity_score</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>similarity_measure</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>see_also</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>other</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>comment</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="3">
-    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"Not"</formula1>
-    </dataValidation>
-    <dataValidation sqref="S2:S1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"owl class,owl object property,owl data property,owl annotation property,owl named individual,skos concept,rdfs resource,rdfs class,rdfs literal,rdfs datatype,rdf property"</formula1>
-    </dataValidation>
-    <dataValidation sqref="X2:X1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"1:1,1:n,n:1,1:0,0:1,n:n"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1120,7 +909,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1163,6 +952,37 @@
       <c r="F1" t="inlineStr">
         <is>
           <t>local_name</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>prefix_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>prefix_url</t>
         </is>
       </c>
     </row>
@@ -1231,4 +1051,22 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Re-generate all schema-derived files.
This is simply the result of `poetry run make all`.
</commit_message>
<xml_diff>
--- a/project/excel/sssom_schema.xlsx
+++ b/project/excel/sssom_schema.xlsx
@@ -14,7 +14,8 @@
     <sheet name="prefix" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="extension definition" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="Propagatable" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="NoTermFound" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Versionable" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="NoTermFound" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -420,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD1"/>
+  <dimension ref="A1:AL1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -431,162 +432,208 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>sssom_version</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>curie_map</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>mappings</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>mapping_set_id</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>mapping_set_version</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>mapping_set_source</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>mapping_set_title</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>mapping_set_description</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>mapping_set_confidence</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
         <is>
           <t>creator_id</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>creator_label</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>license</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>subject_type</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>subject_source</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>subject_source_version</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>object_type</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>object_source</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>object_source_version</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>predicate_type</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
         <is>
           <t>mapping_provider</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>cardinality_scope</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
         <is>
           <t>mapping_tool</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>mapping_tool_id</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
         <is>
           <t>mapping_tool_version</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>mapping_date</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>publication_date</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>subject_match_field</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>object_match_field</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>subject_preprocessing</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>object_preprocessing</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>similarity_measure</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>curation_rule</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>curation_rule_text</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
         <is>
           <t>see_also</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>issue_tracker</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>other</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>comment</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>extension_definitions</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation sqref="K2:K1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"owl class,owl object property,owl data property,owl annotation property,owl named individual,skos concept,rdfs resource,rdfs class,rdfs literal,rdfs datatype,rdf property"</formula1>
+  <dataValidations count="4">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"1.0,1.1"</formula1>
     </dataValidation>
-    <dataValidation sqref="N2:N1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"owl class,owl object property,owl data property,owl annotation property,owl named individual,skos concept,rdfs resource,rdfs class,rdfs literal,rdfs datatype,rdf property"</formula1>
+    <dataValidation sqref="M2:M1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"owl class,owl object property,owl data property,owl annotation property,owl named individual,skos concept,rdfs resource,rdfs class,rdfs literal,rdfs datatype,rdf property,composed entity expression"</formula1>
+    </dataValidation>
+    <dataValidation sqref="P2:P1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"owl class,owl object property,owl data property,owl annotation property,owl named individual,skos concept,rdfs resource,rdfs class,rdfs literal,rdfs datatype,rdf property,composed entity expression"</formula1>
+    </dataValidation>
+    <dataValidation sqref="S2:S1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"owl class,owl object property,owl data property,owl annotation property,owl named individual,skos concept,rdfs resource,rdfs class,rdfs literal,rdfs datatype,rdf property,composed entity expression"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -599,7 +646,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AR1"/>
+  <dimension ref="A1:AV1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -610,238 +657,261 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>record_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>subject_id</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>subject_label</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>subject_category</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>predicate_id</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>predicate_label</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>predicate_modifier</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>object_id</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>object_label</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>object_category</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>mapping_justification</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>author_id</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>author_label</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>reviewer_id</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>reviewer_label</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>creator_id</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>creator_label</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>license</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>subject_type</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>subject_source</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>subject_source_version</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>object_type</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>object_source</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>object_source_version</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>predicate_type</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
         <is>
           <t>mapping_provider</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>mapping_source</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>mapping_cardinality</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>cardinality_scope</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
         <is>
           <t>mapping_tool</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>mapping_tool_id</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
         <is>
           <t>mapping_tool_version</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>mapping_date</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>publication_date</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>confidence</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>curation_rule</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>curation_rule_text</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>subject_match_field</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>object_match_field</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>match_string</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>subject_preprocessing</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>object_preprocessing</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>similarity_score</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>similarity_measure</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>see_also</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>issue_tracker_item</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>other</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>comment</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+  <dataValidations count="5">
+    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"Not"</formula1>
     </dataValidation>
-    <dataValidation sqref="R2:R1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"owl class,owl object property,owl data property,owl annotation property,owl named individual,skos concept,rdfs resource,rdfs class,rdfs literal,rdfs datatype,rdf property"</formula1>
+    <dataValidation sqref="S2:S1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"owl class,owl object property,owl data property,owl annotation property,owl named individual,skos concept,rdfs resource,rdfs class,rdfs literal,rdfs datatype,rdf property,composed entity expression"</formula1>
     </dataValidation>
-    <dataValidation sqref="U2:U1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"owl class,owl object property,owl data property,owl annotation property,owl named individual,skos concept,rdfs resource,rdfs class,rdfs literal,rdfs datatype,rdf property"</formula1>
+    <dataValidation sqref="V2:V1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"owl class,owl object property,owl data property,owl annotation property,owl named individual,skos concept,rdfs resource,rdfs class,rdfs literal,rdfs datatype,rdf property,composed entity expression"</formula1>
     </dataValidation>
-    <dataValidation sqref="Z2:Z1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"1:1,1:n,n:1,1:0,0:1,n:n"</formula1>
+    <dataValidation sqref="Y2:Y1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"owl class,owl object property,owl data property,owl annotation property,owl named individual,skos concept,rdfs resource,rdfs class,rdfs literal,rdfs datatype,rdf property,composed entity expression"</formula1>
+    </dataValidation>
+    <dataValidation sqref="AB2:AB1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"1:1,1:n,n:1,n:n,1:0,0:1,0:0"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1066,6 +1136,37 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>added_in</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"1.0,1.1"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update generated files (#497)
Resolves [#496]

- [x] `docs/` have been added/updated if necessary
- [x] `make test` has been run locally
- ~~[ ] tests have been added/updated (if applicable)~~
- ~~[ ]
[CHANGELOG.md](https://github.com/mapping-commons/sssom/blob/master/CHANGELOG.md)
has been updated.~~

This PR:

* re-generates all the schema-derived files so that they reflect the
latest changes made to the schema;
* adds some notes in the CONTRIBUTING document about how to make a SSSOM
release, and in particular to remind the person doing the release that
schema-derived files must be re-generated before a release.
</commit_message>
<xml_diff>
--- a/project/excel/sssom_schema.xlsx
+++ b/project/excel/sssom_schema.xlsx
@@ -14,7 +14,8 @@
     <sheet name="prefix" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="extension definition" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="Propagatable" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="NoTermFound" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Versionable" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="NoTermFound" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -420,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD1"/>
+  <dimension ref="A1:AL1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -431,162 +432,208 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>sssom_version</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>curie_map</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>mappings</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>mapping_set_id</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>mapping_set_version</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>mapping_set_source</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>mapping_set_title</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>mapping_set_description</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>mapping_set_confidence</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
         <is>
           <t>creator_id</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>creator_label</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>license</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>subject_type</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>subject_source</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>subject_source_version</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>object_type</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>object_source</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>object_source_version</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>predicate_type</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
         <is>
           <t>mapping_provider</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>cardinality_scope</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
         <is>
           <t>mapping_tool</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>mapping_tool_id</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
         <is>
           <t>mapping_tool_version</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>mapping_date</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>publication_date</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>subject_match_field</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>object_match_field</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>subject_preprocessing</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>object_preprocessing</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>similarity_measure</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>curation_rule</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>curation_rule_text</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
         <is>
           <t>see_also</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>issue_tracker</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>other</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>comment</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>extension_definitions</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation sqref="K2:K1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"owl class,owl object property,owl data property,owl annotation property,owl named individual,skos concept,rdfs resource,rdfs class,rdfs literal,rdfs datatype,rdf property"</formula1>
+  <dataValidations count="4">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"1.0,1.1"</formula1>
     </dataValidation>
-    <dataValidation sqref="N2:N1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"owl class,owl object property,owl data property,owl annotation property,owl named individual,skos concept,rdfs resource,rdfs class,rdfs literal,rdfs datatype,rdf property"</formula1>
+    <dataValidation sqref="M2:M1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"owl class,owl object property,owl data property,owl annotation property,owl named individual,skos concept,rdfs resource,rdfs class,rdfs literal,rdfs datatype,rdf property,composed entity expression"</formula1>
+    </dataValidation>
+    <dataValidation sqref="P2:P1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"owl class,owl object property,owl data property,owl annotation property,owl named individual,skos concept,rdfs resource,rdfs class,rdfs literal,rdfs datatype,rdf property,composed entity expression"</formula1>
+    </dataValidation>
+    <dataValidation sqref="S2:S1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"owl class,owl object property,owl data property,owl annotation property,owl named individual,skos concept,rdfs resource,rdfs class,rdfs literal,rdfs datatype,rdf property,composed entity expression"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -599,7 +646,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AR1"/>
+  <dimension ref="A1:AV1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -610,238 +657,261 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>record_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>subject_id</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>subject_label</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>subject_category</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>predicate_id</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>predicate_label</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>predicate_modifier</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>object_id</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>object_label</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>object_category</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>mapping_justification</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>author_id</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>author_label</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>reviewer_id</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>reviewer_label</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>creator_id</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>creator_label</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>license</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>subject_type</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>subject_source</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>subject_source_version</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>object_type</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>object_source</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>object_source_version</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>predicate_type</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
         <is>
           <t>mapping_provider</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>mapping_source</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>mapping_cardinality</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>cardinality_scope</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
         <is>
           <t>mapping_tool</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>mapping_tool_id</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
         <is>
           <t>mapping_tool_version</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>mapping_date</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>publication_date</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>confidence</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>curation_rule</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>curation_rule_text</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>subject_match_field</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>object_match_field</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>match_string</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>subject_preprocessing</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>object_preprocessing</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>similarity_score</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>similarity_measure</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>see_also</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>issue_tracker_item</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>other</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>comment</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+  <dataValidations count="5">
+    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"Not"</formula1>
     </dataValidation>
-    <dataValidation sqref="R2:R1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"owl class,owl object property,owl data property,owl annotation property,owl named individual,skos concept,rdfs resource,rdfs class,rdfs literal,rdfs datatype,rdf property"</formula1>
+    <dataValidation sqref="S2:S1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"owl class,owl object property,owl data property,owl annotation property,owl named individual,skos concept,rdfs resource,rdfs class,rdfs literal,rdfs datatype,rdf property,composed entity expression"</formula1>
     </dataValidation>
-    <dataValidation sqref="U2:U1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"owl class,owl object property,owl data property,owl annotation property,owl named individual,skos concept,rdfs resource,rdfs class,rdfs literal,rdfs datatype,rdf property"</formula1>
+    <dataValidation sqref="V2:V1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"owl class,owl object property,owl data property,owl annotation property,owl named individual,skos concept,rdfs resource,rdfs class,rdfs literal,rdfs datatype,rdf property,composed entity expression"</formula1>
     </dataValidation>
-    <dataValidation sqref="Z2:Z1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"1:1,1:n,n:1,1:0,0:1,n:n"</formula1>
+    <dataValidation sqref="Y2:Y1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"owl class,owl object property,owl data property,owl annotation property,owl named individual,skos concept,rdfs resource,rdfs class,rdfs literal,rdfs datatype,rdf property,composed entity expression"</formula1>
+    </dataValidation>
+    <dataValidation sqref="AB2:AB1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"1:1,1:n,n:1,n:n,1:0,0:1,0:0"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1066,6 +1136,37 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>added_in</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"1.0,1.1"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>